<commit_message>
new property and excel file
</commit_message>
<xml_diff>
--- a/com.tyss.studentmanagementframework/src/test/resources/StudentManagement.xlsx
+++ b/com.tyss.studentmanagementframework/src/test/resources/StudentManagement.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fd8f0ac56cb2c71/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F28BD52F-1E7A-42BE-A864-6BC07E139595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F62F839-9D1D-4040-A177-5D7C3FBD7F35}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4185"/>
   </bookViews>
   <sheets>
     <sheet name="Classroom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Tc_Id</t>
   </si>
@@ -50,12 +45,30 @@
   </si>
   <si>
     <t>Search</t>
+  </si>
+  <si>
+    <t>addstudent dropdown</t>
+  </si>
+  <si>
+    <t>Grade 1</t>
+  </si>
+  <si>
+    <t>Grade 2</t>
+  </si>
+  <si>
+    <t>Grade 3</t>
+  </si>
+  <si>
+    <t>LKG</t>
+  </si>
+  <si>
+    <t>UKG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,20 +413,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C79AA5-8234-4F13-BF01-B15408781F23}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +440,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -440,10 +457,36 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>